<commit_message>
Added demo for IEEEVC.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_ieeevc.xlsx
+++ b/andes/cases/ieee14/ieee14_ieeevc.xlsx
@@ -8,33 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1880F07-7301-EF43-A1EF-F97CCF430FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57FC94C-CAF6-214F-86B2-8474346C2619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33400" yWindow="5640" windowWidth="26040" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IEEEVC" sheetId="15" r:id="rId1"/>
     <sheet name="IEEET1" sheetId="14" r:id="rId2"/>
-    <sheet name="Toggler" sheetId="1" r:id="rId3"/>
-    <sheet name="Bus" sheetId="2" r:id="rId4"/>
-    <sheet name="PQ" sheetId="3" r:id="rId5"/>
-    <sheet name="PV" sheetId="4" r:id="rId6"/>
-    <sheet name="Slack" sheetId="5" r:id="rId7"/>
-    <sheet name="Shunt" sheetId="6" r:id="rId8"/>
-    <sheet name="Line" sheetId="7" r:id="rId9"/>
-    <sheet name="Area" sheetId="8" r:id="rId10"/>
-    <sheet name="GENROU" sheetId="9" r:id="rId11"/>
-    <sheet name="TGOV1" sheetId="10" r:id="rId12"/>
-    <sheet name="EXST1" sheetId="11" r:id="rId13"/>
-    <sheet name="ESST3A" sheetId="12" r:id="rId14"/>
-    <sheet name="BusFreq" sheetId="13" r:id="rId15"/>
+    <sheet name="ESST3A" sheetId="12" r:id="rId3"/>
+    <sheet name="Toggler" sheetId="1" r:id="rId4"/>
+    <sheet name="Bus" sheetId="2" r:id="rId5"/>
+    <sheet name="PQ" sheetId="3" r:id="rId6"/>
+    <sheet name="PV" sheetId="4" r:id="rId7"/>
+    <sheet name="Slack" sheetId="5" r:id="rId8"/>
+    <sheet name="Shunt" sheetId="6" r:id="rId9"/>
+    <sheet name="Line" sheetId="7" r:id="rId10"/>
+    <sheet name="Area" sheetId="8" r:id="rId11"/>
+    <sheet name="GENROU" sheetId="9" r:id="rId12"/>
+    <sheet name="TGOV1" sheetId="10" r:id="rId13"/>
+    <sheet name="BusFreq" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="181">
   <si>
     <t>idx</t>
   </si>
@@ -483,9 +482,6 @@
     <t>TF</t>
   </si>
   <si>
-    <t>EXST1_1</t>
-  </si>
-  <si>
     <t>KM</t>
   </si>
   <si>
@@ -577,13 +573,16 @@
   </si>
   <si>
     <t>xc</t>
+  </si>
+  <si>
+    <t>IEEEVC_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,6 +594,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -992,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FEF9996-4A48-B04C-ADB7-43291DFB4911}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1014,13 +1019,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1028,22 +1033,1436 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F2">
         <v>0.05</v>
       </c>
       <c r="G2">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3">
+        <v>0.05</v>
+      </c>
+      <c r="G3">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:X21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="I2">
+        <v>69</v>
+      </c>
+      <c r="J2">
+        <v>69</v>
+      </c>
+      <c r="K2">
+        <v>1.9380000000000001E-2</v>
+      </c>
+      <c r="L2">
+        <v>5.917E-2</v>
+      </c>
+      <c r="M2">
+        <v>5.28E-2</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3">
+        <v>69</v>
+      </c>
+      <c r="J3">
+        <v>69</v>
+      </c>
+      <c r="K3">
+        <v>5.4030000000000002E-2</v>
+      </c>
+      <c r="L3">
+        <v>0.22303999999999999</v>
+      </c>
+      <c r="M3">
+        <v>4.9200000000000001E-2</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>69</v>
+      </c>
+      <c r="J4">
+        <v>69</v>
+      </c>
+      <c r="K4">
+        <v>4.6989999999999997E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.19797000000000001</v>
+      </c>
+      <c r="M4">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+      <c r="I5">
+        <v>69</v>
+      </c>
+      <c r="J5">
+        <v>69</v>
+      </c>
+      <c r="K5">
+        <v>5.8110000000000002E-2</v>
+      </c>
+      <c r="L5">
+        <v>0.17632</v>
+      </c>
+      <c r="M5">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
+      <c r="I6">
+        <v>69</v>
+      </c>
+      <c r="J6">
+        <v>69</v>
+      </c>
+      <c r="K6">
+        <v>5.6950000000000001E-2</v>
+      </c>
+      <c r="L6">
+        <v>0.17388000000000001</v>
+      </c>
+      <c r="M6">
+        <v>3.4599999999999999E-2</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+      <c r="I7">
+        <v>69</v>
+      </c>
+      <c r="J7">
+        <v>69</v>
+      </c>
+      <c r="K7">
+        <v>6.701E-2</v>
+      </c>
+      <c r="L7">
+        <v>0.17102999999999999</v>
+      </c>
+      <c r="M7">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>60</v>
+      </c>
+      <c r="I8">
+        <v>69</v>
+      </c>
+      <c r="J8">
+        <v>69</v>
+      </c>
+      <c r="K8">
+        <v>1.3350000000000001E-2</v>
+      </c>
+      <c r="L8">
+        <v>4.2110000000000002E-2</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>60</v>
+      </c>
+      <c r="I9">
+        <v>138</v>
+      </c>
+      <c r="J9">
+        <v>138</v>
+      </c>
+      <c r="K9">
+        <v>9.4979999999999995E-2</v>
+      </c>
+      <c r="L9">
+        <v>0.19889999999999999</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <v>60</v>
+      </c>
+      <c r="I10">
+        <v>138</v>
+      </c>
+      <c r="J10">
+        <v>138</v>
+      </c>
+      <c r="K10">
+        <v>0.12291000000000001</v>
+      </c>
+      <c r="L10">
+        <v>0.25580999999999998</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>60</v>
+      </c>
+      <c r="I11">
+        <v>138</v>
+      </c>
+      <c r="J11">
+        <v>138</v>
+      </c>
+      <c r="K11">
+        <v>6.615E-2</v>
+      </c>
+      <c r="L11">
+        <v>0.13027</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>100</v>
+      </c>
+      <c r="H12">
+        <v>60</v>
+      </c>
+      <c r="I12">
+        <v>138</v>
+      </c>
+      <c r="J12">
+        <v>138</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0.11001</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>60</v>
+      </c>
+      <c r="I13">
+        <v>138</v>
+      </c>
+      <c r="J13">
+        <v>138</v>
+      </c>
+      <c r="K13">
+        <v>3.1809999999999998E-2</v>
+      </c>
+      <c r="L13">
+        <v>8.4500000000000006E-2</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>60</v>
+      </c>
+      <c r="I14">
+        <v>138</v>
+      </c>
+      <c r="J14">
+        <v>138</v>
+      </c>
+      <c r="K14">
+        <v>0.12711</v>
+      </c>
+      <c r="L14">
+        <v>0.27038000000000001</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>11</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>60</v>
+      </c>
+      <c r="I15">
+        <v>138</v>
+      </c>
+      <c r="J15">
+        <v>138</v>
+      </c>
+      <c r="K15">
+        <v>8.2049999999999998E-2</v>
+      </c>
+      <c r="L15">
+        <v>0.19206999999999999</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16">
+        <v>12</v>
+      </c>
+      <c r="F16">
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+      <c r="H16">
+        <v>60</v>
+      </c>
+      <c r="I16">
+        <v>138</v>
+      </c>
+      <c r="J16">
+        <v>138</v>
+      </c>
+      <c r="K16">
+        <v>0.22092000000000001</v>
+      </c>
+      <c r="L16">
+        <v>0.19988</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17">
+        <v>13</v>
+      </c>
+      <c r="F17">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>60</v>
+      </c>
+      <c r="I17">
+        <v>138</v>
+      </c>
+      <c r="J17">
+        <v>138</v>
+      </c>
+      <c r="K17">
+        <v>0.17093</v>
+      </c>
+      <c r="L17">
+        <v>0.34802</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>100</v>
+      </c>
+      <c r="H18">
+        <v>60</v>
+      </c>
+      <c r="I18">
+        <v>69</v>
+      </c>
+      <c r="J18">
+        <v>138</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0.20912</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>0.99677000000000004</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>9</v>
+      </c>
+      <c r="G19">
+        <v>100</v>
+      </c>
+      <c r="H19">
+        <v>60</v>
+      </c>
+      <c r="I19">
+        <v>69</v>
+      </c>
+      <c r="J19">
+        <v>138</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0.55618000000000001</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>0.99677000000000004</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+      <c r="H20">
+        <v>60</v>
+      </c>
+      <c r="I20">
+        <v>138</v>
+      </c>
+      <c r="J20">
+        <v>69</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0.25202000000000002</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>0.99677000000000004</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="H21">
+        <v>60</v>
+      </c>
+      <c r="I21">
+        <v>69</v>
+      </c>
+      <c r="J21">
+        <v>138</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0.17615</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>0.99677000000000004</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1051,7 +2470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1109,7 +2528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
@@ -1662,7 +3081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
@@ -1927,465 +3346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:Q2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2">
-        <v>0.02</v>
-      </c>
-      <c r="G2">
-        <v>99</v>
-      </c>
-      <c r="H2">
-        <v>-99</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0.02</v>
-      </c>
-      <c r="K2">
-        <v>50</v>
-      </c>
-      <c r="L2">
-        <v>0.02</v>
-      </c>
-      <c r="M2">
-        <v>9999</v>
-      </c>
-      <c r="N2">
-        <v>-9999</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0.01</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:Z4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2">
-        <v>0.02</v>
-      </c>
-      <c r="G2">
-        <v>0.2</v>
-      </c>
-      <c r="H2">
-        <v>-0.2</v>
-      </c>
-      <c r="I2">
-        <v>8</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>5</v>
-      </c>
-      <c r="L2">
-        <v>20</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>99</v>
-      </c>
-      <c r="O2">
-        <v>-99</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>3.67</v>
-      </c>
-      <c r="R2">
-        <v>0.435</v>
-      </c>
-      <c r="S2">
-        <v>5.48</v>
-      </c>
-      <c r="T2">
-        <v>0.01</v>
-      </c>
-      <c r="U2">
-        <v>9.7999999999999997E-3</v>
-      </c>
-      <c r="V2">
-        <v>3.86</v>
-      </c>
-      <c r="W2">
-        <v>3.33</v>
-      </c>
-      <c r="X2">
-        <v>0.4</v>
-      </c>
-      <c r="Y2">
-        <v>99</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F3">
-        <v>0.02</v>
-      </c>
-      <c r="G3">
-        <v>0.2</v>
-      </c>
-      <c r="H3">
-        <v>-0.2</v>
-      </c>
-      <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>5</v>
-      </c>
-      <c r="L3">
-        <v>20</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>99</v>
-      </c>
-      <c r="O3">
-        <v>-99</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>3.67</v>
-      </c>
-      <c r="R3">
-        <v>0.435</v>
-      </c>
-      <c r="S3">
-        <v>5.48</v>
-      </c>
-      <c r="T3">
-        <v>0.01</v>
-      </c>
-      <c r="U3">
-        <v>9.7999999999999997E-3</v>
-      </c>
-      <c r="V3">
-        <v>3.86</v>
-      </c>
-      <c r="W3">
-        <v>3.33</v>
-      </c>
-      <c r="X3">
-        <v>0.4</v>
-      </c>
-      <c r="Y3">
-        <v>99</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4">
-        <v>0.02</v>
-      </c>
-      <c r="G4">
-        <v>0.2</v>
-      </c>
-      <c r="H4">
-        <v>-0.2</v>
-      </c>
-      <c r="I4">
-        <v>8</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>5</v>
-      </c>
-      <c r="L4">
-        <v>20</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>99</v>
-      </c>
-      <c r="O4">
-        <v>-99</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>3.67</v>
-      </c>
-      <c r="R4">
-        <v>0.435</v>
-      </c>
-      <c r="S4">
-        <v>5.48</v>
-      </c>
-      <c r="T4">
-        <v>0.01</v>
-      </c>
-      <c r="U4">
-        <v>9.7999999999999997E-3</v>
-      </c>
-      <c r="V4">
-        <v>3.86</v>
-      </c>
-      <c r="W4">
-        <v>3.33</v>
-      </c>
-      <c r="X4">
-        <v>0.4</v>
-      </c>
-      <c r="Y4">
-        <v>99</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -2413,10 +3374,10 @@
         <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>59</v>
@@ -2427,13 +3388,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -2453,13 +3414,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2479,13 +3440,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2548,10 +3509,10 @@
         <v>145</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>147</v>
@@ -2560,19 +3521,19 @@
         <v>148</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -2580,13 +3541,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E2" t="s">
         <v>121</v>
@@ -2598,6 +3559,342 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:Z4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2">
+        <v>0.02</v>
+      </c>
+      <c r="G2">
+        <v>0.2</v>
+      </c>
+      <c r="H2">
+        <v>-0.2</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>99</v>
+      </c>
+      <c r="O2">
+        <v>-99</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>3.67</v>
+      </c>
+      <c r="R2">
+        <v>0.435</v>
+      </c>
+      <c r="S2">
+        <v>5.48</v>
+      </c>
+      <c r="T2">
+        <v>0.01</v>
+      </c>
+      <c r="U2">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="V2">
+        <v>3.86</v>
+      </c>
+      <c r="W2">
+        <v>3.33</v>
+      </c>
+      <c r="X2">
+        <v>0.4</v>
+      </c>
+      <c r="Y2">
+        <v>99</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3">
+        <v>0.02</v>
+      </c>
+      <c r="G3">
+        <v>0.2</v>
+      </c>
+      <c r="H3">
+        <v>-0.2</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>20</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>99</v>
+      </c>
+      <c r="O3">
+        <v>-99</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>3.67</v>
+      </c>
+      <c r="R3">
+        <v>0.435</v>
+      </c>
+      <c r="S3">
+        <v>5.48</v>
+      </c>
+      <c r="T3">
+        <v>0.01</v>
+      </c>
+      <c r="U3">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="V3">
+        <v>3.86</v>
+      </c>
+      <c r="W3">
+        <v>3.33</v>
+      </c>
+      <c r="X3">
+        <v>0.4</v>
+      </c>
+      <c r="Y3">
+        <v>99</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4">
+        <v>0.02</v>
+      </c>
+      <c r="G4">
+        <v>0.2</v>
+      </c>
+      <c r="H4">
+        <v>-0.2</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>99</v>
+      </c>
+      <c r="O4">
+        <v>-99</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>3.67</v>
+      </c>
+      <c r="R4">
+        <v>0.435</v>
+      </c>
+      <c r="S4">
+        <v>5.48</v>
+      </c>
+      <c r="T4">
+        <v>0.01</v>
+      </c>
+      <c r="U4">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="V4">
+        <v>3.86</v>
+      </c>
+      <c r="W4">
+        <v>3.33</v>
+      </c>
+      <c r="X4">
+        <v>0.4</v>
+      </c>
+      <c r="Y4">
+        <v>99</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2682,7 +3979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N15"/>
   <sheetViews>
@@ -3358,7 +4655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -3794,7 +5091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
@@ -4093,7 +5390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -4230,7 +5527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -4340,1394 +5637,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:X21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2">
-        <v>60</v>
-      </c>
-      <c r="I2">
-        <v>69</v>
-      </c>
-      <c r="J2">
-        <v>69</v>
-      </c>
-      <c r="K2">
-        <v>1.9380000000000001E-2</v>
-      </c>
-      <c r="L2">
-        <v>5.917E-2</v>
-      </c>
-      <c r="M2">
-        <v>5.28E-2</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3">
-        <v>60</v>
-      </c>
-      <c r="I3">
-        <v>69</v>
-      </c>
-      <c r="J3">
-        <v>69</v>
-      </c>
-      <c r="K3">
-        <v>5.4030000000000002E-2</v>
-      </c>
-      <c r="L3">
-        <v>0.22303999999999999</v>
-      </c>
-      <c r="M3">
-        <v>4.9200000000000001E-2</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-      <c r="H4">
-        <v>60</v>
-      </c>
-      <c r="I4">
-        <v>69</v>
-      </c>
-      <c r="J4">
-        <v>69</v>
-      </c>
-      <c r="K4">
-        <v>4.6989999999999997E-2</v>
-      </c>
-      <c r="L4">
-        <v>0.19797000000000001</v>
-      </c>
-      <c r="M4">
-        <v>4.3799999999999999E-2</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5">
-        <v>60</v>
-      </c>
-      <c r="I5">
-        <v>69</v>
-      </c>
-      <c r="J5">
-        <v>69</v>
-      </c>
-      <c r="K5">
-        <v>5.8110000000000002E-2</v>
-      </c>
-      <c r="L5">
-        <v>0.17632</v>
-      </c>
-      <c r="M5">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>100</v>
-      </c>
-      <c r="H6">
-        <v>60</v>
-      </c>
-      <c r="I6">
-        <v>69</v>
-      </c>
-      <c r="J6">
-        <v>69</v>
-      </c>
-      <c r="K6">
-        <v>5.6950000000000001E-2</v>
-      </c>
-      <c r="L6">
-        <v>0.17388000000000001</v>
-      </c>
-      <c r="M6">
-        <v>3.4599999999999999E-2</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>100</v>
-      </c>
-      <c r="H7">
-        <v>60</v>
-      </c>
-      <c r="I7">
-        <v>69</v>
-      </c>
-      <c r="J7">
-        <v>69</v>
-      </c>
-      <c r="K7">
-        <v>6.701E-2</v>
-      </c>
-      <c r="L7">
-        <v>0.17102999999999999</v>
-      </c>
-      <c r="M7">
-        <v>1.2800000000000001E-2</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="G8">
-        <v>100</v>
-      </c>
-      <c r="H8">
-        <v>60</v>
-      </c>
-      <c r="I8">
-        <v>69</v>
-      </c>
-      <c r="J8">
-        <v>69</v>
-      </c>
-      <c r="K8">
-        <v>1.3350000000000001E-2</v>
-      </c>
-      <c r="L8">
-        <v>4.2110000000000002E-2</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-      <c r="F9">
-        <v>11</v>
-      </c>
-      <c r="G9">
-        <v>100</v>
-      </c>
-      <c r="H9">
-        <v>60</v>
-      </c>
-      <c r="I9">
-        <v>138</v>
-      </c>
-      <c r="J9">
-        <v>138</v>
-      </c>
-      <c r="K9">
-        <v>9.4979999999999995E-2</v>
-      </c>
-      <c r="L9">
-        <v>0.19889999999999999</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10">
-        <v>6</v>
-      </c>
-      <c r="F10">
-        <v>12</v>
-      </c>
-      <c r="G10">
-        <v>100</v>
-      </c>
-      <c r="H10">
-        <v>60</v>
-      </c>
-      <c r="I10">
-        <v>138</v>
-      </c>
-      <c r="J10">
-        <v>138</v>
-      </c>
-      <c r="K10">
-        <v>0.12291000000000001</v>
-      </c>
-      <c r="L10">
-        <v>0.25580999999999998</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11">
-        <v>6</v>
-      </c>
-      <c r="F11">
-        <v>13</v>
-      </c>
-      <c r="G11">
-        <v>100</v>
-      </c>
-      <c r="H11">
-        <v>60</v>
-      </c>
-      <c r="I11">
-        <v>138</v>
-      </c>
-      <c r="J11">
-        <v>138</v>
-      </c>
-      <c r="K11">
-        <v>6.615E-2</v>
-      </c>
-      <c r="L11">
-        <v>0.13027</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>1</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12">
-        <v>7</v>
-      </c>
-      <c r="F12">
-        <v>9</v>
-      </c>
-      <c r="G12">
-        <v>100</v>
-      </c>
-      <c r="H12">
-        <v>60</v>
-      </c>
-      <c r="I12">
-        <v>138</v>
-      </c>
-      <c r="J12">
-        <v>138</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0.11001</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>1</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13">
-        <v>9</v>
-      </c>
-      <c r="F13">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>100</v>
-      </c>
-      <c r="H13">
-        <v>60</v>
-      </c>
-      <c r="I13">
-        <v>138</v>
-      </c>
-      <c r="J13">
-        <v>138</v>
-      </c>
-      <c r="K13">
-        <v>3.1809999999999998E-2</v>
-      </c>
-      <c r="L13">
-        <v>8.4500000000000006E-2</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>1</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14">
-        <v>9</v>
-      </c>
-      <c r="F14">
-        <v>14</v>
-      </c>
-      <c r="G14">
-        <v>100</v>
-      </c>
-      <c r="H14">
-        <v>60</v>
-      </c>
-      <c r="I14">
-        <v>138</v>
-      </c>
-      <c r="J14">
-        <v>138</v>
-      </c>
-      <c r="K14">
-        <v>0.12711</v>
-      </c>
-      <c r="L14">
-        <v>0.27038000000000001</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>1</v>
-      </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15">
-        <v>10</v>
-      </c>
-      <c r="F15">
-        <v>11</v>
-      </c>
-      <c r="G15">
-        <v>100</v>
-      </c>
-      <c r="H15">
-        <v>60</v>
-      </c>
-      <c r="I15">
-        <v>138</v>
-      </c>
-      <c r="J15">
-        <v>138</v>
-      </c>
-      <c r="K15">
-        <v>8.2049999999999998E-2</v>
-      </c>
-      <c r="L15">
-        <v>0.19206999999999999</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16">
-        <v>12</v>
-      </c>
-      <c r="F16">
-        <v>13</v>
-      </c>
-      <c r="G16">
-        <v>100</v>
-      </c>
-      <c r="H16">
-        <v>60</v>
-      </c>
-      <c r="I16">
-        <v>138</v>
-      </c>
-      <c r="J16">
-        <v>138</v>
-      </c>
-      <c r="K16">
-        <v>0.22092000000000001</v>
-      </c>
-      <c r="L16">
-        <v>0.19988</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17">
-        <v>13</v>
-      </c>
-      <c r="F17">
-        <v>14</v>
-      </c>
-      <c r="G17">
-        <v>100</v>
-      </c>
-      <c r="H17">
-        <v>60</v>
-      </c>
-      <c r="I17">
-        <v>138</v>
-      </c>
-      <c r="J17">
-        <v>138</v>
-      </c>
-      <c r="K17">
-        <v>0.17093</v>
-      </c>
-      <c r="L17">
-        <v>0.34802</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>1</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18">
-        <v>4</v>
-      </c>
-      <c r="F18">
-        <v>7</v>
-      </c>
-      <c r="G18">
-        <v>100</v>
-      </c>
-      <c r="H18">
-        <v>60</v>
-      </c>
-      <c r="I18">
-        <v>69</v>
-      </c>
-      <c r="J18">
-        <v>138</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0.20912</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>1</v>
-      </c>
-      <c r="T18">
-        <v>0.99677000000000004</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19">
-        <v>4</v>
-      </c>
-      <c r="F19">
-        <v>9</v>
-      </c>
-      <c r="G19">
-        <v>100</v>
-      </c>
-      <c r="H19">
-        <v>60</v>
-      </c>
-      <c r="I19">
-        <v>69</v>
-      </c>
-      <c r="J19">
-        <v>138</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0.55618000000000001</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
-      <c r="T19">
-        <v>0.99677000000000004</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20">
-        <v>6</v>
-      </c>
-      <c r="F20">
-        <v>5</v>
-      </c>
-      <c r="G20">
-        <v>100</v>
-      </c>
-      <c r="H20">
-        <v>60</v>
-      </c>
-      <c r="I20">
-        <v>138</v>
-      </c>
-      <c r="J20">
-        <v>69</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0.25202000000000002</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>1</v>
-      </c>
-      <c r="T20">
-        <v>0.99677000000000004</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21">
-        <v>8</v>
-      </c>
-      <c r="F21">
-        <v>7</v>
-      </c>
-      <c r="G21">
-        <v>100</v>
-      </c>
-      <c r="H21">
-        <v>60</v>
-      </c>
-      <c r="I21">
-        <v>69</v>
-      </c>
-      <c r="J21">
-        <v>138</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0.17615</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-      <c r="T21">
-        <v>0.99677000000000004</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>